<commit_message>
adding FNLC and combining det his
</commit_message>
<xml_diff>
--- a/occ_mod_tracking.xlsx
+++ b/occ_mod_tracking.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caraappel/Documents/_RESEARCH/Activity centers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B564AD3-4C93-0F4C-AAAB-D53A348DDD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5A12E9-EEA9-4E47-85AB-5E989D014F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{991A3EA2-37E0-E74B-BBA6-A89020C75055}"/>
+    <workbookView xWindow="-34280" yWindow="2180" windowWidth="28040" windowHeight="17440" xr2:uid="{991A3EA2-37E0-E74B-BBA6-A89020C75055}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="single-season" sheetId="1" r:id="rId1"/>
+    <sheet name="single-season multi-state" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,19 +37,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>model</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>response_variable</t>
+  </si>
+  <si>
+    <t>psi_covar</t>
+  </si>
+  <si>
+    <t>p_covar</t>
+  </si>
+  <si>
+    <t>any_STOC</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>effort_site</t>
+  </si>
+  <si>
+    <t>dist_actual</t>
+  </si>
+  <si>
+    <t>dist_actual + site</t>
+  </si>
+  <si>
+    <t>dist_actual + nest</t>
+  </si>
+  <si>
+    <t>female_4NLC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -62,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +119,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,20 +450,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14E5D6B-5CB9-6442-BDFC-26C7BA818D97}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>2021</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>2021</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89547C0A-D686-4148-ABBB-ADAAE0D382AD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>